<commit_message>
Ejecucion de los casos de pruebas
</commit_message>
<xml_diff>
--- a/Documentación/TercerHito/CasosDePrueba/CasosDePrueba.xlsx
+++ b/Documentación/TercerHito/CasosDePrueba/CasosDePrueba.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Trezza\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1EE8737-8CED-4039-8CA5-BE5D1221B520}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
   <si>
     <t>Objetivo</t>
   </si>
@@ -166,13 +160,329 @@
   </si>
   <si>
     <t>ingresar datos personales</t>
+  </si>
+  <si>
+    <t>Resultado obtenido</t>
+  </si>
+  <si>
+    <t>Planilla de excel completa sin logear</t>
+  </si>
+  <si>
+    <t>Planilla de excel completa legeado</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bueno.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Mensaje de error: Necesita estar logueado para crear aula. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bueno.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Mensaje de error: Necesita estar logueado para matricular. </t>
+    </r>
+  </si>
+  <si>
+    <t>Carga de datos correctos estando logeado</t>
+  </si>
+  <si>
+    <t>Carga de datos con caracteres incorrectos</t>
+  </si>
+  <si>
+    <t>Carga de datos correctos sin estar logeado</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bueno.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Mensaje de error: Necesita estar logueado para reutilizar aula</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Malo.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Matricula exitosamente pero muesta el Error: Internal Server Error.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Malo.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Crea el aula pero no manda mail y muestra el Error: Bad request</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bueno</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>. No modifica el aula y muestra un mesaje de error en el campo donde se encuentra</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bueno.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> No crea el aula y muestra un mesaje de error en el campo donde se encuentra.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bueno.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Mensaje de error: Necesita estar logueado para eliminar aula</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bueno.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> No elimina el aula y muestra un mesaje de error en el campo donde se encuentra</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Malo.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Error: Bad request, no manda mail pero modifica el aula</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Malo.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Error: Bad request, no manda mail pero elimina el aula</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Regular.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> No muestra ningun mensaje de error personalizado solo el error: Bad request.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Malo.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Error: Bad request, no manda mail y no crea la capacitación </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bueno.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> agrega un microtaller y envia mail correctamente</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bueno. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>agrega un microtaller y envia mail correctamente</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Regular.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> agrega un microtaller y envia mail correctamente incluso con caracteres incorrectos</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -190,6 +500,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -222,7 +538,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -232,6 +548,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,7 +611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -344,7 +663,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -538,18 +857,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -557,12 +876,13 @@
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="2" width="35.28515625" customWidth="1"/>
     <col min="3" max="3" width="51.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" customWidth="1"/>
     <col min="5" max="5" width="42.85546875" customWidth="1"/>
-    <col min="6" max="256" width="10" customWidth="1"/>
+    <col min="6" max="6" width="82.42578125" customWidth="1"/>
+    <col min="7" max="256" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
@@ -578,8 +898,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -596,7 +919,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -613,7 +936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -623,11 +946,17 @@
       <c r="C4" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="E4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -637,11 +966,17 @@
       <c r="C5" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="E5" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -651,11 +986,17 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -665,11 +1006,17 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
+      <c r="D7" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E7" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -679,11 +1026,17 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -693,11 +1046,17 @@
       <c r="C9" t="s">
         <v>43</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -707,11 +1066,17 @@
       <c r="C10" t="s">
         <v>43</v>
       </c>
+      <c r="D10" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E10" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -721,11 +1086,17 @@
       <c r="C11" t="s">
         <v>43</v>
       </c>
+      <c r="D11" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="E11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
@@ -735,11 +1106,17 @@
       <c r="C12" t="s">
         <v>44</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
@@ -749,11 +1126,17 @@
       <c r="C13" t="s">
         <v>44</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E13" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
@@ -763,11 +1146,17 @@
       <c r="C14" t="s">
         <v>44</v>
       </c>
+      <c r="D14" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="E14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>14</v>
       </c>
@@ -777,11 +1166,17 @@
       <c r="C15" t="s">
         <v>45</v>
       </c>
+      <c r="D15" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>15</v>
       </c>
@@ -791,11 +1186,17 @@
       <c r="C16" t="s">
         <v>45</v>
       </c>
+      <c r="D16" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E16" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>16</v>
       </c>
@@ -805,11 +1206,17 @@
       <c r="C17" t="s">
         <v>45</v>
       </c>
+      <c r="D17" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="E17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>17</v>
       </c>
@@ -819,11 +1226,17 @@
       <c r="C18" t="s">
         <v>46</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>18</v>
       </c>
@@ -833,11 +1246,17 @@
       <c r="C19" t="s">
         <v>46</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E19" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>19</v>
       </c>
@@ -847,8 +1266,14 @@
       <c r="C20" t="s">
         <v>46</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="E20" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>